<commit_message>
dodalem jezyki w koncu tak aby mozna bylo zmieniac na 3 jezyki ktore dodalem jak narazie, zostalo zrobic tak aby dalo sie cofnac do wyboru jezyka w ustawieniach i zeby na tryb ciemny sie dalo ustawic i zeby to cos sie pojawialo raz i tyle
</commit_message>
<xml_diff>
--- a/app/src/main/assets/slowa.xlsx
+++ b/app/src/main/assets/slowa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boy12\AndroidStudioProjects\HiraganaAndKatakana\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2595B5B-54A9-421F-8354-A6BADC6E2D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A44AC3-C0BA-4227-95E2-DAC5056C2270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{658EBC5A-91B2-430A-B88F-08BE90825D71}"/>
   </bookViews>
@@ -381,15 +381,6 @@
     <t>Romaji</t>
   </si>
   <si>
-    <t>Polskie</t>
-  </si>
-  <si>
-    <t>Angielskie</t>
-  </si>
-  <si>
-    <t>Hiszpańskie</t>
-  </si>
-  <si>
     <t>Kategoria</t>
   </si>
   <si>
@@ -2119,6 +2110,15 @@
   </si>
   <si>
     <t>history</t>
+  </si>
+  <si>
+    <t>Polski</t>
+  </si>
+  <si>
+    <t>Angielski</t>
+  </si>
+  <si>
+    <t>Hiszpański</t>
   </si>
 </sst>
 </file>
@@ -2489,8 +2489,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J138" sqref="J138"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2503,116 +2503,116 @@
         <v>113</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2632,7 +2632,7 @@
         <v>93</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2652,7 +2652,7 @@
         <v>98</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2672,27 +2672,27 @@
         <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2703,16 +2703,16 @@
         <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2726,13 +2726,13 @@
         <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2752,27 +2752,27 @@
         <v>108</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2792,27 +2792,27 @@
         <v>103</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2826,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2846,53 +2846,53 @@
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2912,7 +2912,7 @@
         <v>83</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2926,13 +2926,13 @@
         <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2946,33 +2946,33 @@
         <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -2986,13 +2986,13 @@
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -3006,13 +3006,13 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -3026,18 +3026,18 @@
         <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -3046,113 +3046,113 @@
         <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3166,13 +3166,13 @@
         <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3186,133 +3186,133 @@
         <v>62</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3326,13 +3326,13 @@
         <v>13</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3346,13 +3346,13 @@
         <v>16</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3366,53 +3366,53 @@
         <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3426,481 +3426,481 @@
         <v>10</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="F50" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="F53" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="E56" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="F59" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="F61" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>342</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="F63" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="F64" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="F65" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>362</v>
-      </c>
       <c r="F66" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>367</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="F68" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="F69" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="F70" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>109</v>
@@ -3912,7 +3912,7 @@
         <v>111</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -3923,16 +3923,16 @@
         <v>67</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -3943,116 +3943,116 @@
         <v>69</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>396</v>
-      </c>
       <c r="F74" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>401</v>
-      </c>
       <c r="F75" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>406</v>
-      </c>
       <c r="F76" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="F77" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>416</v>
-      </c>
       <c r="F78" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4063,16 +4063,16 @@
         <v>73</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -4083,136 +4083,136 @@
         <v>54</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="F81" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>432</v>
-      </c>
       <c r="F82" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>437</v>
-      </c>
       <c r="F83" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>441</v>
-      </c>
       <c r="E84" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="F85" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="E86" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="F86" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -4226,13 +4226,13 @@
         <v>55</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4246,93 +4246,93 @@
         <v>52</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="E91" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>468</v>
-      </c>
       <c r="F91" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -4346,473 +4346,473 @@
         <v>49</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>479</v>
-      </c>
       <c r="F95" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>484</v>
-      </c>
       <c r="F96" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>489</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="F98" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>501</v>
-      </c>
       <c r="F100" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>505</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="F104" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>520</v>
-      </c>
       <c r="F105" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>525</v>
-      </c>
       <c r="F106" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>536</v>
-      </c>
       <c r="F108" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>540</v>
-      </c>
       <c r="E109" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>544</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>548</v>
-      </c>
       <c r="E111" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>553</v>
-      </c>
       <c r="F112" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>561</v>
-      </c>
       <c r="F114" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="E116" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>569</v>
-      </c>
       <c r="F116" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4823,196 +4823,196 @@
         <v>78</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>577</v>
-      </c>
       <c r="F118" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>582</v>
-      </c>
       <c r="F119" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="E120" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>587</v>
-      </c>
       <c r="F120" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>592</v>
-      </c>
       <c r="F121" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>599</v>
-      </c>
       <c r="F123" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="E124" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>604</v>
-      </c>
       <c r="F124" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="E125" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>609</v>
-      </c>
       <c r="F125" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>416</v>
-      </c>
       <c r="F126" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5026,33 +5026,33 @@
         <v>65</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="E128" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>617</v>
-      </c>
       <c r="F128" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5066,13 +5066,13 @@
         <v>43</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5086,53 +5086,53 @@
         <v>46</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>626</v>
-      </c>
       <c r="F131" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>631</v>
-      </c>
       <c r="F132" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5146,73 +5146,73 @@
         <v>40</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="E134" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>638</v>
-      </c>
       <c r="F134" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>643</v>
-      </c>
       <c r="F135" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="E136" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>648</v>
-      </c>
       <c r="F136" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -5226,193 +5226,193 @@
         <v>76</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="E138" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>655</v>
-      </c>
       <c r="F138" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="E139" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>660</v>
-      </c>
       <c r="F139" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="E140" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>665</v>
-      </c>
       <c r="F140" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="E141" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>670</v>
-      </c>
       <c r="F141" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>674</v>
-      </c>
       <c r="E142" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="E143" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>679</v>
-      </c>
       <c r="F143" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="E144" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>684</v>
-      </c>
       <c r="F144" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="E145" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>689</v>
-      </c>
       <c r="F145" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>693</v>
-      </c>
       <c r="E146" s="1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ogarnalem switcha do hiragany basic ktory zmienia jezyki
</commit_message>
<xml_diff>
--- a/app/src/main/assets/slowa.xlsx
+++ b/app/src/main/assets/slowa.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boy12\AndroidStudioProjects\HiraganaAndKatakana\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A44AC3-C0BA-4227-95E2-DAC5056C2270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5E6BDF-CFAC-4173-AB7D-736C5383FA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{658EBC5A-91B2-430A-B88F-08BE90825D71}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{658EBC5A-91B2-430A-B88F-08BE90825D71}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$1:$F$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$1:$F$146</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2486,16 +2486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C73CE1-289B-4850-BEA5-2E91E0C14A7D}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="H1" sqref="H1:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -2514,8 +2513,14 @@
       <c r="F1" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
@@ -2534,8 +2539,14 @@
       <c r="F2" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -2554,8 +2565,14 @@
       <c r="F3" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -2574,8 +2591,14 @@
       <c r="F4" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
@@ -2594,8 +2617,14 @@
       <c r="F5" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -2614,8 +2643,14 @@
       <c r="F6" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>89</v>
       </c>
@@ -2634,8 +2669,14 @@
       <c r="F7" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>94</v>
       </c>
@@ -2654,8 +2695,14 @@
       <c r="F8" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -2674,8 +2721,14 @@
       <c r="F9" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -2694,8 +2747,14 @@
       <c r="F10" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2714,8 +2773,14 @@
       <c r="F11" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2734,8 +2799,14 @@
       <c r="F12" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -2754,8 +2825,14 @@
       <c r="F13" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>150</v>
       </c>
@@ -2774,8 +2851,14 @@
       <c r="F14" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -2794,8 +2877,14 @@
       <c r="F15" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>155</v>
       </c>
@@ -2814,8 +2903,14 @@
       <c r="F16" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2834,8 +2929,14 @@
       <c r="F17" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -2854,8 +2955,14 @@
       <c r="F18" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>164</v>
       </c>
@@ -2874,8 +2981,14 @@
       <c r="F19" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>169</v>
       </c>
@@ -2894,8 +3007,14 @@
       <c r="F20" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -2914,8 +3033,14 @@
       <c r="F21" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2934,8 +3059,14 @@
       <c r="F22" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -2954,8 +3085,14 @@
       <c r="F23" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>178</v>
       </c>
@@ -2974,8 +3111,14 @@
       <c r="F24" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2994,8 +3137,14 @@
       <c r="F25" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -3014,8 +3163,14 @@
       <c r="F26" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
@@ -3034,8 +3189,14 @@
       <c r="F27" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>191</v>
       </c>
@@ -3054,8 +3215,14 @@
       <c r="F28" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>194</v>
       </c>
@@ -3074,8 +3241,14 @@
       <c r="F29" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>199</v>
       </c>
@@ -3094,8 +3267,14 @@
       <c r="F30" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>204</v>
       </c>
@@ -3114,8 +3293,14 @@
       <c r="F31" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -3134,8 +3319,14 @@
       <c r="F32" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>214</v>
       </c>
@@ -3154,8 +3345,14 @@
       <c r="F33" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -3175,7 +3372,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>60</v>
       </c>
@@ -3195,7 +3392,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>223</v>
       </c>
@@ -3215,7 +3412,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>228</v>
       </c>
@@ -3235,7 +3432,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>233</v>
       </c>
@@ -3255,7 +3452,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>238</v>
       </c>
@@ -3275,7 +3472,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>243</v>
       </c>
@@ -3295,7 +3492,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>248</v>
       </c>
@@ -3315,7 +3512,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -3335,7 +3532,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3552,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -3375,7 +3572,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>260</v>
       </c>
@@ -3395,7 +3592,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>265</v>
       </c>
@@ -3415,7 +3612,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -3435,7 +3632,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>272</v>
       </c>
@@ -3455,7 +3652,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>277</v>
       </c>
@@ -3475,7 +3672,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>282</v>
       </c>
@@ -3495,7 +3692,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>287</v>
       </c>
@@ -3515,7 +3712,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>292</v>
       </c>
@@ -3535,7 +3732,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>297</v>
       </c>
@@ -3555,7 +3752,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>302</v>
       </c>
@@ -3575,7 +3772,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>307</v>
       </c>
@@ -3595,7 +3792,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>312</v>
       </c>
@@ -3615,7 +3812,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>316</v>
       </c>
@@ -3635,7 +3832,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>318</v>
       </c>
@@ -3655,7 +3852,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>321</v>
       </c>
@@ -3675,7 +3872,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>326</v>
       </c>
@@ -3695,7 +3892,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>331</v>
       </c>
@@ -3715,7 +3912,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>335</v>
       </c>
@@ -3735,7 +3932,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>340</v>
       </c>
@@ -3755,7 +3952,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>345</v>
       </c>
@@ -3775,7 +3972,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>350</v>
       </c>
@@ -3795,7 +3992,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>355</v>
       </c>
@@ -3815,7 +4012,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>360</v>
       </c>
@@ -3835,7 +4032,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>365</v>
       </c>
@@ -3855,7 +4052,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>370</v>
       </c>
@@ -3875,7 +4072,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>375</v>
       </c>
@@ -3895,7 +4092,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>380</v>
       </c>
@@ -5646,14 +5843,7 @@
       <c r="A204" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F86" xr:uid="{18C73CE1-289B-4850-BEA5-2E91E0C14A7D}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="hobby"/>
-        <filter val="rośliny"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F146" xr:uid="{18C73CE1-289B-4850-BEA5-2E91E0C14A7D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>